<commit_message>
Fundamentos de Sociologia - Tarea 4
</commit_message>
<xml_diff>
--- a/Plan_Ingenieria_Informatica.xlsx
+++ b/Plan_Ingenieria_Informatica.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jrodrigue253\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jrodrigue253\Github\UNED\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D1B3E7-5D60-44E8-86CC-5140B08CC6A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2E1B1C9-B050-4E9D-8B45-CB56C2A01D40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7965" windowWidth="29040" windowHeight="15840" xr2:uid="{8230E5AE-A8B0-403C-B098-7F142039F630}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8230E5AE-A8B0-403C-B098-7F142039F630}"/>
   </bookViews>
   <sheets>
     <sheet name="Diplomado" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="83">
   <si>
     <t>Bloque</t>
   </si>
@@ -278,6 +278,12 @@
   </si>
   <si>
     <t>Pasantía de Licenciatura en Ingeniería Informática (Semestral)</t>
+  </si>
+  <si>
+    <t>Nota Final</t>
+  </si>
+  <si>
+    <t>#</t>
   </si>
 </sst>
 </file>
@@ -334,7 +340,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -366,6 +372,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -681,444 +693,543 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD8781F1-B9E9-4C62-8830-019F772FBC45}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="1"/>
-    <col min="2" max="2" width="28.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625" style="1"/>
+    <col min="3" max="3" width="28.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>3</v>
-      </c>
       <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
+      <c r="I1" s="12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="C2" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="6">
-        <v>3</v>
-      </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="10" t="s">
+      <c r="D2" s="6">
+        <v>3</v>
+      </c>
+      <c r="E2" s="6"/>
+      <c r="F2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="10"/>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="6"/>
+      <c r="H2" s="11" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
+      <c r="I2" s="10"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="C3" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="6">
-        <v>3</v>
-      </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="10"/>
+      <c r="D3" s="6">
+        <v>3</v>
+      </c>
+      <c r="E3" s="6"/>
       <c r="F3" s="10"/>
-      <c r="G3" s="11"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G3" s="6"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="10"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6">
         <v>3304</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="C4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="6">
+      <c r="D4" s="6">
         <v>4</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="6"/>
+      <c r="F4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G4" s="6"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6">
         <v>3068</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="C5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="6">
-        <v>3</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="10"/>
+      <c r="D5" s="6">
+        <v>3</v>
+      </c>
+      <c r="E5" s="6"/>
       <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G5" s="6"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6">
         <v>997</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="C6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="6">
-        <v>3</v>
-      </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="10"/>
+      <c r="D6" s="6">
+        <v>3</v>
+      </c>
+      <c r="E6" s="6"/>
       <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G6" s="6"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6">
         <v>4038</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="C7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="6">
-        <v>3</v>
-      </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="10"/>
+      <c r="D7" s="6">
+        <v>3</v>
+      </c>
+      <c r="E7" s="6"/>
       <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G7" s="6"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6">
         <v>3071</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="C8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="6">
-        <v>3</v>
-      </c>
       <c r="D8" s="6">
+        <v>3</v>
+      </c>
+      <c r="E8" s="6">
         <v>3304</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="F8" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G8" s="6"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6">
         <v>3069</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="C9" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="6">
-        <v>3</v>
-      </c>
       <c r="D9" s="6">
+        <v>3</v>
+      </c>
+      <c r="E9" s="6">
         <v>3068</v>
       </c>
-      <c r="E9" s="10"/>
       <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G9" s="6"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6">
         <v>3072</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="C10" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="6">
-        <v>3</v>
-      </c>
       <c r="D10" s="6">
+        <v>3</v>
+      </c>
+      <c r="E10" s="6">
         <v>997</v>
       </c>
-      <c r="E10" s="10"/>
       <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="6"/>
-      <c r="B11" s="10" t="s">
+      <c r="G10" s="6"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="6">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="6">
-        <v>3</v>
-      </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="10"/>
+      <c r="D11" s="6">
+        <v>3</v>
+      </c>
+      <c r="E11" s="6"/>
       <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G11" s="6"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6">
         <v>831</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="C12" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="6">
+      <c r="D12" s="6">
         <v>4</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="E12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="F12" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G12" s="6"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="6">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6">
         <v>823</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="C13" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="6">
+      <c r="D13" s="6">
         <v>4</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="E13" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="F13" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G13" s="6"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="6">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6">
         <v>226</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="C14" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="6">
+      <c r="D14" s="6">
         <v>4</v>
       </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="10"/>
+      <c r="E14" s="6"/>
       <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G14" s="6"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="6">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6">
         <v>104</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="C15" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="6">
+      <c r="D15" s="6">
         <v>4</v>
       </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="10"/>
+      <c r="E15" s="6"/>
       <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G15" s="6"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="6">
+        <v>15</v>
+      </c>
+      <c r="B16" s="6">
         <v>824</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="C16" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="6">
+      <c r="D16" s="6">
         <v>4</v>
       </c>
-      <c r="D16" s="6">
+      <c r="E16" s="6">
         <v>831</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="F16" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G16" s="6"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="6">
+        <v>16</v>
+      </c>
+      <c r="B17" s="6">
         <v>826</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="C17" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="6">
-        <v>3</v>
-      </c>
       <c r="D17" s="6">
+        <v>3</v>
+      </c>
+      <c r="E17" s="6">
         <v>831</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="F17" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="G17" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="10"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="6">
+        <v>17</v>
+      </c>
+      <c r="B18" s="6">
         <v>3306</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="C18" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="6">
+      <c r="D18" s="6">
         <v>4</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="E18" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="F18" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G18" s="6"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="6">
+        <v>18</v>
+      </c>
+      <c r="B19" s="6">
         <v>883</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="C19" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="6">
-        <v>3</v>
-      </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="6">
+        <v>3</v>
+      </c>
+      <c r="E19" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="F19" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="6"/>
-      <c r="B20" s="10" t="s">
+      <c r="G19" s="6"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20" s="6">
+        <v>19</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="6">
-        <v>3</v>
-      </c>
-      <c r="D20" s="6"/>
-      <c r="E20" s="10"/>
+      <c r="D20" s="6">
+        <v>3</v>
+      </c>
+      <c r="E20" s="6"/>
       <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G20" s="6"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="6">
+        <v>20</v>
+      </c>
+      <c r="B21" s="6">
         <v>3300</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="C21" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="6">
+      <c r="D21" s="6">
         <v>4</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="E21" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="F21" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G21" s="6"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="6">
+        <v>21</v>
+      </c>
+      <c r="B22" s="6">
         <v>830</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="C22" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="6">
+      <c r="D22" s="6">
         <v>4</v>
       </c>
-      <c r="D22" s="6">
+      <c r="E22" s="6">
         <v>824826</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="F22" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G22" s="6"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="6">
+        <v>22</v>
+      </c>
+      <c r="B23" s="6">
         <v>825</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="C23" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="6">
-        <v>3</v>
-      </c>
       <c r="D23" s="6">
+        <v>3</v>
+      </c>
+      <c r="E23" s="6">
         <v>824</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="F23" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="G23" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G23" s="10"/>
-    </row>
-    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+    </row>
+    <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="6">
+        <v>23</v>
+      </c>
+      <c r="B24" s="6">
         <v>881</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="C24" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="6">
-        <v>3</v>
-      </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="6">
+        <v>3</v>
+      </c>
+      <c r="E24" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="F24" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1128,303 +1239,352 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA12924-F294-4484-86F1-E460BC0E3C72}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="38.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
         <v>3301</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
         <v>3075</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="1">
-        <v>3</v>
-      </c>
       <c r="D3" s="1">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1">
         <v>830</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="1">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
         <v>3307</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4" s="1">
         <v>4</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C5" s="1">
-        <v>3</v>
-      </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="1">
+        <v>3</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="1">
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
         <v>3302</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6" s="1">
         <v>4</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>3301</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="1">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
         <v>3084</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="1">
-        <v>3</v>
-      </c>
       <c r="D7" s="1">
+        <v>3</v>
+      </c>
+      <c r="E7" s="1">
         <v>826</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="1">
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="6">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
         <v>3308</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="1">
+      <c r="D8" s="1">
         <v>4</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <v>3306</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="1">
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="6">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
         <v>3070</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="1">
-        <v>3</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="1">
+        <v>3</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="1">
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="6">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
         <v>3076</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="1">
-        <v>3</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="1">
+        <v>3</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="1">
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="6">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
         <v>3305</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="1">
+      <c r="D11" s="1">
         <v>4</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="1">
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="6">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
         <v>3029</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="1">
-        <v>3</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="1">
+        <v>3</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="6">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="1">
-        <v>3</v>
-      </c>
-      <c r="D13" s="1"/>
+      <c r="D13" s="1">
+        <v>3</v>
+      </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="1">
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="6">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
         <v>3073</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C14" s="1">
-        <v>3</v>
-      </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="1">
+        <v>3</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="1">
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="6">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
         <v>3077</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C15" s="1">
-        <v>3</v>
-      </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1" t="s">
+      <c r="D15" s="1">
+        <v>3</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="1">
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="6">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
         <v>886</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="1">
+      <c r="D16" s="1">
         <v>4</v>
       </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="1"/>
+      <c r="F16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1617,12 +1777,12 @@
       <c r="A12" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>

</xml_diff>

<commit_message>
20212C - Matematicas para Computacion 1
</commit_message>
<xml_diff>
--- a/Plan_Ingenieria_Informatica.xlsx
+++ b/Plan_Ingenieria_Informatica.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jrodrigue253\Github\UNED\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A09D30B5-4D02-4D49-8877-0A736C269651}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C17B813-CD15-45D9-936D-3FE946032347}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2400" windowWidth="29040" windowHeight="15840" xr2:uid="{8230E5AE-A8B0-403C-B098-7F142039F630}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8230E5AE-A8B0-403C-B098-7F142039F630}"/>
   </bookViews>
   <sheets>
     <sheet name="Diplomado" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="83">
   <si>
     <t>Bloque</t>
   </si>
@@ -299,7 +299,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -309,6 +309,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -340,7 +346,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -363,9 +369,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -373,15 +376,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -699,7 +715,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -739,32 +755,34 @@
       <c r="H1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="10" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="6">
+      <c r="A2" s="13">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="6">
-        <v>3</v>
-      </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="9" t="s">
+      <c r="D2" s="13">
+        <v>3</v>
+      </c>
+      <c r="E2" s="13"/>
+      <c r="F2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="10" t="s">
+      <c r="G2" s="13"/>
+      <c r="H2" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="I2" s="9"/>
+      <c r="I2" s="16">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
@@ -773,17 +791,17 @@
       <c r="B3" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>36</v>
       </c>
       <c r="D3" s="6">
         <v>3</v>
       </c>
       <c r="E3" s="6"/>
-      <c r="F3" s="9"/>
+      <c r="F3" s="8"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="8"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
@@ -792,38 +810,40 @@
       <c r="B4" s="6">
         <v>3304</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="6">
         <v>4</v>
       </c>
       <c r="E4" s="6"/>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="8" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="6"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="6">
+      <c r="A5" s="17">
         <v>4</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="17">
         <v>3068</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="6">
-        <v>3</v>
-      </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
+      <c r="D5" s="17">
+        <v>3</v>
+      </c>
+      <c r="E5" s="17"/>
+      <c r="F5" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="17"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
@@ -832,17 +852,17 @@
       <c r="B6" s="6">
         <v>997</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="6">
         <v>3</v>
       </c>
       <c r="E6" s="6"/>
-      <c r="F6" s="9"/>
+      <c r="F6" s="8"/>
       <c r="G6" s="6"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
@@ -851,17 +871,17 @@
       <c r="B7" s="6">
         <v>4038</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="8" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="6">
         <v>3</v>
       </c>
       <c r="E7" s="6"/>
-      <c r="F7" s="9"/>
+      <c r="F7" s="8"/>
       <c r="G7" s="6"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
@@ -870,7 +890,7 @@
       <c r="B8" s="6">
         <v>3071</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="6">
@@ -879,12 +899,12 @@
       <c r="E8" s="6">
         <v>3304</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="8" t="s">
         <v>8</v>
       </c>
       <c r="G8" s="6"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
@@ -893,7 +913,7 @@
       <c r="B9" s="6">
         <v>3069</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="6">
@@ -902,10 +922,10 @@
       <c r="E9" s="6">
         <v>3068</v>
       </c>
-      <c r="F9" s="9"/>
+      <c r="F9" s="8"/>
       <c r="G9" s="6"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
@@ -914,7 +934,7 @@
       <c r="B10" s="6">
         <v>3072</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="8" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="6">
@@ -923,27 +943,27 @@
       <c r="E10" s="6">
         <v>997</v>
       </c>
-      <c r="F10" s="9"/>
+      <c r="F10" s="8"/>
       <c r="G10" s="6"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <v>10</v>
       </c>
       <c r="B11" s="6"/>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="8" t="s">
         <v>15</v>
       </c>
       <c r="D11" s="6">
         <v>3</v>
       </c>
       <c r="E11" s="6"/>
-      <c r="F11" s="9"/>
+      <c r="F11" s="8"/>
       <c r="G11" s="6"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
@@ -952,7 +972,7 @@
       <c r="B12" s="6">
         <v>831</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="8" t="s">
         <v>16</v>
       </c>
       <c r="D12" s="6">
@@ -961,12 +981,12 @@
       <c r="E12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="8" t="s">
         <v>18</v>
       </c>
       <c r="G12" s="6"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="6">
@@ -975,7 +995,7 @@
       <c r="B13" s="6">
         <v>823</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="8" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="6">
@@ -984,12 +1004,12 @@
       <c r="E13" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="8" t="s">
         <v>8</v>
       </c>
       <c r="G13" s="6"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="6">
@@ -998,17 +1018,17 @@
       <c r="B14" s="6">
         <v>226</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="8" t="s">
         <v>21</v>
       </c>
       <c r="D14" s="6">
         <v>4</v>
       </c>
       <c r="E14" s="6"/>
-      <c r="F14" s="9"/>
+      <c r="F14" s="8"/>
       <c r="G14" s="6"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="6">
@@ -1017,17 +1037,17 @@
       <c r="B15" s="6">
         <v>104</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="8" t="s">
         <v>22</v>
       </c>
       <c r="D15" s="6">
         <v>4</v>
       </c>
       <c r="E15" s="6"/>
-      <c r="F15" s="9"/>
+      <c r="F15" s="8"/>
       <c r="G15" s="6"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="6">
@@ -1036,7 +1056,7 @@
       <c r="B16" s="6">
         <v>824</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D16" s="6">
@@ -1045,12 +1065,12 @@
       <c r="E16" s="6">
         <v>831</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F16" s="8" t="s">
         <v>18</v>
       </c>
       <c r="G16" s="6"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="6">
@@ -1059,7 +1079,7 @@
       <c r="B17" s="6">
         <v>826</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="8" t="s">
         <v>24</v>
       </c>
       <c r="D17" s="6">
@@ -1068,14 +1088,14 @@
       <c r="E17" s="6">
         <v>831</v>
       </c>
-      <c r="F17" s="9" t="s">
+      <c r="F17" s="8" t="s">
         <v>8</v>
       </c>
       <c r="G17" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="6">
@@ -1084,7 +1104,7 @@
       <c r="B18" s="6">
         <v>3306</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="8" t="s">
         <v>26</v>
       </c>
       <c r="D18" s="6">
@@ -1093,12 +1113,12 @@
       <c r="E18" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="F18" s="8" t="s">
         <v>18</v>
       </c>
       <c r="G18" s="6"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="6">
@@ -1107,7 +1127,7 @@
       <c r="B19" s="6">
         <v>883</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="8" t="s">
         <v>28</v>
       </c>
       <c r="D19" s="6">
@@ -1116,29 +1136,29 @@
       <c r="E19" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="F19" s="8" t="s">
         <v>18</v>
       </c>
       <c r="G19" s="6"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="6">
         <v>19</v>
       </c>
       <c r="B20" s="6"/>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="8" t="s">
         <v>36</v>
       </c>
       <c r="D20" s="6">
         <v>3</v>
       </c>
       <c r="E20" s="6"/>
-      <c r="F20" s="9"/>
+      <c r="F20" s="8"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="6">
@@ -1147,7 +1167,7 @@
       <c r="B21" s="6">
         <v>3300</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="8" t="s">
         <v>29</v>
       </c>
       <c r="D21" s="6">
@@ -1156,12 +1176,12 @@
       <c r="E21" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F21" s="9" t="s">
+      <c r="F21" s="8" t="s">
         <v>18</v>
       </c>
       <c r="G21" s="6"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="6">
@@ -1170,21 +1190,21 @@
       <c r="B22" s="6">
         <v>830</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="8" t="s">
         <v>31</v>
       </c>
       <c r="D22" s="6">
         <v>4</v>
       </c>
-      <c r="E22" s="13">
+      <c r="E22" s="11">
         <v>824826</v>
       </c>
-      <c r="F22" s="9" t="s">
+      <c r="F22" s="8" t="s">
         <v>18</v>
       </c>
       <c r="G22" s="6"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="6">
@@ -1193,7 +1213,7 @@
       <c r="B23" s="6">
         <v>825</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="8" t="s">
         <v>32</v>
       </c>
       <c r="D23" s="6">
@@ -1202,14 +1222,14 @@
       <c r="E23" s="6">
         <v>824</v>
       </c>
-      <c r="F23" s="9" t="s">
+      <c r="F23" s="8" t="s">
         <v>8</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
     </row>
     <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="6">
@@ -1218,7 +1238,7 @@
       <c r="B24" s="6">
         <v>881</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="8" t="s">
         <v>33</v>
       </c>
       <c r="D24" s="6">
@@ -1227,12 +1247,12 @@
       <c r="E24" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F24" s="9" t="s">
+      <c r="F24" s="8" t="s">
         <v>18</v>
       </c>
       <c r="G24" s="6"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
UNED - Matematica para computacion I - Foro Academico 4 - respuestas
</commit_message>
<xml_diff>
--- a/Plan_Ingenieria_Informatica.xlsx
+++ b/Plan_Ingenieria_Informatica.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jrodrigue253\Github\UNED\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E063C0-D6C0-41AD-A5E6-6343EFF92E56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BAD7BFC-448D-4B87-AAE7-6B174083450F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8230E5AE-A8B0-403C-B098-7F142039F630}"/>
   </bookViews>
@@ -406,9 +406,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -417,6 +414,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -735,7 +735,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -752,35 +752,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="16" t="s">
+      <c r="D1" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="15" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -1288,7 +1288,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1300,31 +1300,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="16" t="s">
+      <c r="D1" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="15" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1335,7 +1335,7 @@
       <c r="B2" s="5">
         <v>3301</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="17" t="s">
         <v>41</v>
       </c>
       <c r="D2" s="5">
@@ -1358,7 +1358,7 @@
       <c r="B3" s="5">
         <v>3075</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="17" t="s">
         <v>43</v>
       </c>
       <c r="D3" s="5">
@@ -1383,7 +1383,7 @@
       <c r="B4" s="5">
         <v>3307</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="17" t="s">
         <v>44</v>
       </c>
       <c r="D4" s="5">
@@ -1406,7 +1406,7 @@
       <c r="B5" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="17" t="s">
         <v>60</v>
       </c>
       <c r="D5" s="5">
@@ -1425,7 +1425,7 @@
       <c r="B6" s="5">
         <v>3302</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="17" t="s">
         <v>46</v>
       </c>
       <c r="D6" s="5">
@@ -1450,7 +1450,7 @@
       <c r="B7" s="5">
         <v>3084</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="17" t="s">
         <v>47</v>
       </c>
       <c r="D7" s="5">
@@ -1473,7 +1473,7 @@
       <c r="B8" s="5">
         <v>3308</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="17" t="s">
         <v>48</v>
       </c>
       <c r="D8" s="5">
@@ -1496,7 +1496,7 @@
       <c r="B9" s="5">
         <v>3070</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="17" t="s">
         <v>49</v>
       </c>
       <c r="D9" s="5">
@@ -1519,7 +1519,7 @@
       <c r="B10" s="5">
         <v>3076</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="17" t="s">
         <v>51</v>
       </c>
       <c r="D10" s="5">
@@ -1542,7 +1542,7 @@
       <c r="B11" s="5">
         <v>3305</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="17" t="s">
         <v>53</v>
       </c>
       <c r="D11" s="5">
@@ -1565,7 +1565,7 @@
       <c r="B12" s="5">
         <v>3029</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="17" t="s">
         <v>55</v>
       </c>
       <c r="D12" s="5">
@@ -1588,7 +1588,7 @@
       <c r="B13" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="17" t="s">
         <v>60</v>
       </c>
       <c r="D13" s="5">
@@ -1607,7 +1607,7 @@
       <c r="B14" s="5">
         <v>3073</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="17" t="s">
         <v>57</v>
       </c>
       <c r="D14" s="5">
@@ -1630,7 +1630,7 @@
       <c r="B15" s="5">
         <v>3077</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="17" t="s">
         <v>59</v>
       </c>
       <c r="D15" s="5">
@@ -1651,7 +1651,7 @@
       <c r="B16" s="5">
         <v>886</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="17" t="s">
         <v>61</v>
       </c>
       <c r="D16" s="5">
@@ -1675,7 +1675,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C3" sqref="C3:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1856,12 +1856,12 @@
       <c r="A12" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>

</xml_diff>

<commit_message>
UNED - Matematica para computacion I - Cuestionario 4 - Solucion
</commit_message>
<xml_diff>
--- a/Plan_Ingenieria_Informatica.xlsx
+++ b/Plan_Ingenieria_Informatica.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jrodrigue253\Github\UNED\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB05585-FF2D-4BB5-B66B-EFC596506DE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B99EB8B-FE15-49EC-8E21-9CC7ABA434A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8230E5AE-A8B0-403C-B098-7F142039F630}"/>
   </bookViews>
@@ -343,12 +343,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -356,6 +350,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -424,7 +424,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -442,9 +442,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -457,14 +454,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -473,47 +466,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -831,584 +828,586 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.6328125" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.6328125" style="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="45" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.81640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.81640625" style="7" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.6328125" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.54296875" customWidth="1"/>
-    <col min="10" max="10" width="9.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.26953125" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="14" t="s">
+      <c r="E1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="11" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="9">
+      <c r="A2" s="21">
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="9">
-        <v>3</v>
-      </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9" t="s">
+      <c r="E2" s="8">
+        <v>3</v>
+      </c>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="9"/>
-      <c r="I2" s="11" t="s">
+      <c r="H2" s="8"/>
+      <c r="I2" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="9">
+      <c r="J2" s="8">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="19">
+      <c r="A3" s="18">
         <v>2</v>
       </c>
       <c r="B3" s="23"/>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="E3" s="19">
-        <v>3</v>
-      </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="19"/>
+      <c r="E3" s="15">
+        <v>3</v>
+      </c>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="15"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="19">
+      <c r="A4" s="18">
         <v>3</v>
       </c>
       <c r="B4" s="23"/>
-      <c r="C4" s="19">
+      <c r="C4" s="15">
         <v>3304</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="15">
         <v>4</v>
       </c>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19" t="s">
+      <c r="F4" s="15"/>
+      <c r="G4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="19"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="19"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="15"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="12">
+      <c r="A5" s="18">
         <v>4</v>
       </c>
       <c r="B5" s="23"/>
-      <c r="C5" s="12">
+      <c r="C5" s="19">
         <v>3068</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="12">
-        <v>3</v>
-      </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12" t="s">
+      <c r="E5" s="19">
+        <v>3</v>
+      </c>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="12"/>
-      <c r="I5" s="13" t="s">
+      <c r="H5" s="19"/>
+      <c r="I5" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="J5" s="12"/>
+      <c r="J5" s="19">
+        <v>9.5</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="19">
+      <c r="A6" s="18">
         <v>5</v>
       </c>
       <c r="B6" s="24"/>
-      <c r="C6" s="19">
+      <c r="C6" s="15">
         <v>997</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="19">
-        <v>3</v>
-      </c>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="19"/>
+      <c r="E6" s="15">
+        <v>3</v>
+      </c>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="15"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="31">
+      <c r="A7" s="18">
         <v>6</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="C7" s="31">
+      <c r="C7" s="27">
         <v>4038</v>
       </c>
-      <c r="D7" s="32" t="s">
+      <c r="D7" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="31">
-        <v>3</v>
-      </c>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="31"/>
+      <c r="E7" s="27">
+        <v>3</v>
+      </c>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="27"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="31">
+      <c r="A8" s="18">
         <v>7</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="31">
+      <c r="B8" s="29"/>
+      <c r="C8" s="27">
         <v>3071</v>
       </c>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="31">
-        <v>3</v>
-      </c>
-      <c r="F8" s="31">
+      <c r="E8" s="27">
+        <v>3</v>
+      </c>
+      <c r="F8" s="27">
         <v>3304</v>
       </c>
-      <c r="G8" s="31" t="s">
+      <c r="G8" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="31"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="31"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="27"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="31">
+      <c r="A9" s="18">
         <v>8</v>
       </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="31">
+      <c r="B9" s="29"/>
+      <c r="C9" s="27">
         <v>3069</v>
       </c>
-      <c r="D9" s="32" t="s">
+      <c r="D9" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="31">
-        <v>3</v>
-      </c>
-      <c r="F9" s="31">
+      <c r="E9" s="27">
+        <v>3</v>
+      </c>
+      <c r="F9" s="27">
         <v>3068</v>
       </c>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="31"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="27"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="31">
+      <c r="A10" s="18">
         <v>9</v>
       </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="31">
+      <c r="B10" s="29"/>
+      <c r="C10" s="27">
         <v>3072</v>
       </c>
-      <c r="D10" s="32" t="s">
+      <c r="D10" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="31">
-        <v>3</v>
-      </c>
-      <c r="F10" s="31">
+      <c r="E10" s="27">
+        <v>3</v>
+      </c>
+      <c r="F10" s="27">
         <v>997</v>
       </c>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="31"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="27"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="31">
+      <c r="A11" s="18">
         <v>10</v>
       </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="32" t="s">
+      <c r="B11" s="30"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="31">
-        <v>3</v>
-      </c>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="31"/>
+      <c r="E11" s="27">
+        <v>3</v>
+      </c>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="27"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="5">
+      <c r="A12" s="18">
         <v>11</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="27">
         <v>831</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="27">
         <v>4</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="5"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="5"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="27"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="5">
+      <c r="A13" s="18">
         <v>12</v>
       </c>
       <c r="B13" s="29"/>
-      <c r="C13" s="5">
+      <c r="C13" s="27">
         <v>823</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="27">
         <v>4</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="5"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="5"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="27"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="5">
+      <c r="A14" s="18">
         <v>13</v>
       </c>
       <c r="B14" s="29"/>
-      <c r="C14" s="5">
+      <c r="C14" s="27">
         <v>226</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="27">
         <v>4</v>
       </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="5"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="27"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="5">
+      <c r="A15" s="18">
         <v>14</v>
       </c>
       <c r="B15" s="30"/>
-      <c r="C15" s="5">
+      <c r="C15" s="27">
         <v>104</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="27">
         <v>4</v>
       </c>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="5"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="27"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="5">
+      <c r="A16" s="18">
         <v>15</v>
       </c>
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="27">
         <v>824</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="27">
         <v>4</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="27">
         <v>831</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="G16" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="5"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="5"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A17" s="5">
+      <c r="A17" s="18">
         <v>16</v>
       </c>
       <c r="B17" s="29"/>
-      <c r="C17" s="5">
+      <c r="C17" s="27">
         <v>826</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="5">
-        <v>3</v>
-      </c>
-      <c r="F17" s="5">
+      <c r="E17" s="27">
+        <v>3</v>
+      </c>
+      <c r="F17" s="27">
         <v>831</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="G17" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="H17" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="I17" s="6"/>
-      <c r="J17" s="5"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="27"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" s="5">
+      <c r="A18" s="18">
         <v>17</v>
       </c>
       <c r="B18" s="29"/>
-      <c r="C18" s="5">
+      <c r="C18" s="27">
         <v>3306</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="27">
         <v>4</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="G18" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="H18" s="5"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="5"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A19" s="5">
+      <c r="A19" s="18">
         <v>18</v>
       </c>
       <c r="B19" s="29"/>
-      <c r="C19" s="5">
+      <c r="C19" s="27">
         <v>883</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="5">
-        <v>3</v>
-      </c>
-      <c r="F19" s="5" t="s">
+      <c r="E19" s="27">
+        <v>3</v>
+      </c>
+      <c r="F19" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="G19" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="H19" s="5"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="5"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="27"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A20" s="5">
+      <c r="A20" s="18">
         <v>19</v>
       </c>
       <c r="B20" s="30"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="6" t="s">
+      <c r="C20" s="27"/>
+      <c r="D20" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="E20" s="5">
-        <v>3</v>
-      </c>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="5"/>
+      <c r="E20" s="27">
+        <v>3</v>
+      </c>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="27"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A21" s="5">
+      <c r="A21" s="18">
         <v>20</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="27">
         <v>3300</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="27">
         <v>4</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F21" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="G21" s="5" t="s">
+      <c r="G21" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="H21" s="5"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="5"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="27"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A22" s="5">
+      <c r="A22" s="18">
         <v>21</v>
       </c>
       <c r="B22" s="29"/>
-      <c r="C22" s="5">
+      <c r="C22" s="27">
         <v>830</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="27">
         <v>4</v>
       </c>
-      <c r="F22" s="7">
+      <c r="F22" s="31">
         <v>824826</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="G22" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="H22" s="5"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="5"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="28"/>
+      <c r="J22" s="27"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A23" s="5">
+      <c r="A23" s="18">
         <v>22</v>
       </c>
       <c r="B23" s="29"/>
-      <c r="C23" s="5">
+      <c r="C23" s="27">
         <v>825</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="E23" s="5">
-        <v>3</v>
-      </c>
-      <c r="F23" s="5">
+      <c r="E23" s="27">
+        <v>3</v>
+      </c>
+      <c r="F23" s="27">
         <v>824</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="G23" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="H23" s="5" t="s">
+      <c r="H23" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="I23" s="6"/>
-      <c r="J23" s="5"/>
+      <c r="I23" s="28"/>
+      <c r="J23" s="27"/>
     </row>
     <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="5">
+      <c r="A24" s="18">
         <v>23</v>
       </c>
       <c r="B24" s="30"/>
-      <c r="C24" s="5">
+      <c r="C24" s="27">
         <v>881</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="E24" s="5">
-        <v>3</v>
-      </c>
-      <c r="F24" s="5" t="s">
+      <c r="E24" s="27">
+        <v>3</v>
+      </c>
+      <c r="F24" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="G24" s="5" t="s">
+      <c r="G24" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="H24" s="5"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="5"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="28"/>
+      <c r="J24" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1440,31 +1439,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="14" t="s">
+      <c r="D1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="11" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1475,7 +1474,7 @@
       <c r="B2" s="5">
         <v>3301</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="13" t="s">
         <v>41</v>
       </c>
       <c r="D2" s="5">
@@ -1498,7 +1497,7 @@
       <c r="B3" s="5">
         <v>3075</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="13" t="s">
         <v>43</v>
       </c>
       <c r="D3" s="5">
@@ -1523,7 +1522,7 @@
       <c r="B4" s="5">
         <v>3307</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="13" t="s">
         <v>44</v>
       </c>
       <c r="D4" s="5">
@@ -1546,7 +1545,7 @@
       <c r="B5" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="13" t="s">
         <v>60</v>
       </c>
       <c r="D5" s="5">
@@ -1565,7 +1564,7 @@
       <c r="B6" s="5">
         <v>3302</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="13" t="s">
         <v>46</v>
       </c>
       <c r="D6" s="5">
@@ -1590,7 +1589,7 @@
       <c r="B7" s="5">
         <v>3084</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="13" t="s">
         <v>47</v>
       </c>
       <c r="D7" s="5">
@@ -1613,7 +1612,7 @@
       <c r="B8" s="5">
         <v>3308</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="13" t="s">
         <v>48</v>
       </c>
       <c r="D8" s="5">
@@ -1636,7 +1635,7 @@
       <c r="B9" s="5">
         <v>3070</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="13" t="s">
         <v>49</v>
       </c>
       <c r="D9" s="5">
@@ -1659,7 +1658,7 @@
       <c r="B10" s="5">
         <v>3076</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="13" t="s">
         <v>51</v>
       </c>
       <c r="D10" s="5">
@@ -1682,7 +1681,7 @@
       <c r="B11" s="5">
         <v>3305</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="13" t="s">
         <v>53</v>
       </c>
       <c r="D11" s="5">
@@ -1705,7 +1704,7 @@
       <c r="B12" s="5">
         <v>3029</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="13" t="s">
         <v>55</v>
       </c>
       <c r="D12" s="5">
@@ -1728,7 +1727,7 @@
       <c r="B13" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="13" t="s">
         <v>60</v>
       </c>
       <c r="D13" s="5">
@@ -1747,7 +1746,7 @@
       <c r="B14" s="5">
         <v>3073</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="13" t="s">
         <v>57</v>
       </c>
       <c r="D14" s="5">
@@ -1770,7 +1769,7 @@
       <c r="B15" s="5">
         <v>3077</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="13" t="s">
         <v>59</v>
       </c>
       <c r="D15" s="5">
@@ -1791,7 +1790,7 @@
       <c r="B16" s="5">
         <v>886</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="13" t="s">
         <v>61</v>
       </c>
       <c r="D16" s="5">
@@ -1996,12 +1995,12 @@
       <c r="A12" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>

</xml_diff>

<commit_message>
UNED - IIIC - 2021
</commit_message>
<xml_diff>
--- a/Plan_Ingenieria_Informatica.xlsx
+++ b/Plan_Ingenieria_Informatica.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jrodrigue253\Github\UNED\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B99EB8B-FE15-49EC-8E21-9CC7ABA434A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1288DBE-9DF7-4AEC-ABFB-F3F6A4579A00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8230E5AE-A8B0-403C-B098-7F142039F630}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="91">
   <si>
     <t>Bloque</t>
   </si>
@@ -305,6 +305,9 @@
   </si>
   <si>
     <t>E</t>
+  </si>
+  <si>
+    <t>IIIC2021</t>
   </si>
 </sst>
 </file>
@@ -328,7 +331,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -356,6 +359,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -424,7 +433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -483,6 +492,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -492,23 +512,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -828,7 +841,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -881,7 +894,7 @@
       <c r="A2" s="21">
         <v>1</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="27" t="s">
         <v>85</v>
       </c>
       <c r="C2" s="9" t="s">
@@ -909,7 +922,7 @@
       <c r="A3" s="18">
         <v>2</v>
       </c>
-      <c r="B3" s="23"/>
+      <c r="B3" s="28"/>
       <c r="C3" s="15" t="s">
         <v>39</v>
       </c>
@@ -929,29 +942,31 @@
       <c r="A4" s="18">
         <v>3</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="15">
+      <c r="B4" s="28"/>
+      <c r="C4" s="25">
         <v>3304</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="25">
         <v>4</v>
       </c>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15" t="s">
+      <c r="F4" s="25"/>
+      <c r="G4" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="15"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="15"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="J4" s="25"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="18">
         <v>4</v>
       </c>
-      <c r="B5" s="23"/>
+      <c r="B5" s="28"/>
       <c r="C5" s="19">
         <v>3068</v>
       </c>
@@ -977,437 +992,439 @@
       <c r="A6" s="18">
         <v>5</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="15">
+      <c r="B6" s="29"/>
+      <c r="C6" s="25">
         <v>997</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="15">
-        <v>3</v>
-      </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="15"/>
+      <c r="E6" s="25">
+        <v>3</v>
+      </c>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="J6" s="25"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="18">
         <v>6</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="C7" s="27">
+      <c r="C7" s="22">
         <v>4038</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="27">
-        <v>3</v>
-      </c>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="27"/>
+      <c r="E7" s="22">
+        <v>3</v>
+      </c>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="22"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="18">
         <v>7</v>
       </c>
-      <c r="B8" s="29"/>
-      <c r="C8" s="27">
+      <c r="B8" s="31"/>
+      <c r="C8" s="22">
         <v>3071</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="27">
-        <v>3</v>
-      </c>
-      <c r="F8" s="27">
+      <c r="E8" s="22">
+        <v>3</v>
+      </c>
+      <c r="F8" s="22">
         <v>3304</v>
       </c>
-      <c r="G8" s="27" t="s">
+      <c r="G8" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="27"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="27"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="22"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="18">
         <v>8</v>
       </c>
-      <c r="B9" s="29"/>
-      <c r="C9" s="27">
+      <c r="B9" s="31"/>
+      <c r="C9" s="22">
         <v>3069</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="27">
-        <v>3</v>
-      </c>
-      <c r="F9" s="27">
+      <c r="E9" s="22">
+        <v>3</v>
+      </c>
+      <c r="F9" s="22">
         <v>3068</v>
       </c>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="27"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="22"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="18">
         <v>9</v>
       </c>
-      <c r="B10" s="29"/>
-      <c r="C10" s="27">
+      <c r="B10" s="31"/>
+      <c r="C10" s="22">
         <v>3072</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="27">
-        <v>3</v>
-      </c>
-      <c r="F10" s="27">
+      <c r="E10" s="22">
+        <v>3</v>
+      </c>
+      <c r="F10" s="22">
         <v>997</v>
       </c>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="27"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="22"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="18">
         <v>10</v>
       </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="28" t="s">
+      <c r="B11" s="32"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="27">
-        <v>3</v>
-      </c>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="27"/>
+      <c r="E11" s="22">
+        <v>3</v>
+      </c>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="22"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="18">
         <v>11</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="C12" s="27">
+      <c r="C12" s="22">
         <v>831</v>
       </c>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="27">
+      <c r="E12" s="22">
         <v>4</v>
       </c>
-      <c r="F12" s="27" t="s">
+      <c r="F12" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="27" t="s">
+      <c r="G12" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="27"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="27"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="22"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="18">
         <v>12</v>
       </c>
-      <c r="B13" s="29"/>
-      <c r="C13" s="27">
+      <c r="B13" s="31"/>
+      <c r="C13" s="22">
         <v>823</v>
       </c>
-      <c r="D13" s="28" t="s">
+      <c r="D13" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="27">
+      <c r="E13" s="22">
         <v>4</v>
       </c>
-      <c r="F13" s="27" t="s">
+      <c r="F13" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="27" t="s">
+      <c r="G13" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="27"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="27"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="22"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="18">
         <v>13</v>
       </c>
-      <c r="B14" s="29"/>
-      <c r="C14" s="27">
+      <c r="B14" s="31"/>
+      <c r="C14" s="22">
         <v>226</v>
       </c>
-      <c r="D14" s="28" t="s">
+      <c r="D14" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="27">
+      <c r="E14" s="22">
         <v>4</v>
       </c>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="27"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="22"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="18">
         <v>14</v>
       </c>
-      <c r="B15" s="30"/>
-      <c r="C15" s="27">
+      <c r="B15" s="32"/>
+      <c r="C15" s="22">
         <v>104</v>
       </c>
-      <c r="D15" s="28" t="s">
+      <c r="D15" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="27">
+      <c r="E15" s="22">
         <v>4</v>
       </c>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="27"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="22"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="18">
         <v>15</v>
       </c>
-      <c r="B16" s="26" t="s">
+      <c r="B16" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="C16" s="27">
+      <c r="C16" s="22">
         <v>824</v>
       </c>
-      <c r="D16" s="28" t="s">
+      <c r="D16" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="27">
+      <c r="E16" s="22">
         <v>4</v>
       </c>
-      <c r="F16" s="27">
+      <c r="F16" s="22">
         <v>831</v>
       </c>
-      <c r="G16" s="27" t="s">
+      <c r="G16" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="27"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="27"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="18">
         <v>16</v>
       </c>
-      <c r="B17" s="29"/>
-      <c r="C17" s="27">
+      <c r="B17" s="31"/>
+      <c r="C17" s="22">
         <v>826</v>
       </c>
-      <c r="D17" s="28" t="s">
+      <c r="D17" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="27">
-        <v>3</v>
-      </c>
-      <c r="F17" s="27">
+      <c r="E17" s="22">
+        <v>3</v>
+      </c>
+      <c r="F17" s="22">
         <v>831</v>
       </c>
-      <c r="G17" s="27" t="s">
+      <c r="G17" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="H17" s="27" t="s">
+      <c r="H17" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="I17" s="28"/>
-      <c r="J17" s="27"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="18">
         <v>17</v>
       </c>
-      <c r="B18" s="29"/>
-      <c r="C18" s="27">
+      <c r="B18" s="31"/>
+      <c r="C18" s="22">
         <v>3306</v>
       </c>
-      <c r="D18" s="28" t="s">
+      <c r="D18" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="27">
+      <c r="E18" s="22">
         <v>4</v>
       </c>
-      <c r="F18" s="27" t="s">
+      <c r="F18" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="G18" s="27" t="s">
+      <c r="G18" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="H18" s="27"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="27"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="18">
         <v>18</v>
       </c>
-      <c r="B19" s="29"/>
-      <c r="C19" s="27">
+      <c r="B19" s="31"/>
+      <c r="C19" s="22">
         <v>883</v>
       </c>
-      <c r="D19" s="28" t="s">
+      <c r="D19" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="27">
-        <v>3</v>
-      </c>
-      <c r="F19" s="27" t="s">
+      <c r="E19" s="22">
+        <v>3</v>
+      </c>
+      <c r="F19" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="G19" s="27" t="s">
+      <c r="G19" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="H19" s="27"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="27"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="22"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="18">
         <v>19</v>
       </c>
-      <c r="B20" s="30"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="28" t="s">
+      <c r="B20" s="32"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="E20" s="27">
-        <v>3</v>
-      </c>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="27"/>
+      <c r="E20" s="22">
+        <v>3</v>
+      </c>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="22"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="18">
         <v>20</v>
       </c>
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="C21" s="27">
+      <c r="C21" s="22">
         <v>3300</v>
       </c>
-      <c r="D21" s="28" t="s">
+      <c r="D21" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E21" s="27">
+      <c r="E21" s="22">
         <v>4</v>
       </c>
-      <c r="F21" s="27" t="s">
+      <c r="F21" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G21" s="27" t="s">
+      <c r="G21" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="H21" s="27"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="27"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="22"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="18">
         <v>21</v>
       </c>
-      <c r="B22" s="29"/>
-      <c r="C22" s="27">
+      <c r="B22" s="31"/>
+      <c r="C22" s="22">
         <v>830</v>
       </c>
-      <c r="D22" s="28" t="s">
+      <c r="D22" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="E22" s="27">
+      <c r="E22" s="22">
         <v>4</v>
       </c>
-      <c r="F22" s="31">
+      <c r="F22" s="24">
         <v>824826</v>
       </c>
-      <c r="G22" s="27" t="s">
+      <c r="G22" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="H22" s="27"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="27"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="22"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="18">
         <v>22</v>
       </c>
-      <c r="B23" s="29"/>
-      <c r="C23" s="27">
+      <c r="B23" s="31"/>
+      <c r="C23" s="22">
         <v>825</v>
       </c>
-      <c r="D23" s="28" t="s">
+      <c r="D23" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E23" s="27">
-        <v>3</v>
-      </c>
-      <c r="F23" s="27">
+      <c r="E23" s="22">
+        <v>3</v>
+      </c>
+      <c r="F23" s="22">
         <v>824</v>
       </c>
-      <c r="G23" s="27" t="s">
+      <c r="G23" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="H23" s="27" t="s">
+      <c r="H23" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="I23" s="28"/>
-      <c r="J23" s="27"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="22"/>
     </row>
     <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="18">
         <v>23</v>
       </c>
-      <c r="B24" s="30"/>
-      <c r="C24" s="27">
+      <c r="B24" s="32"/>
+      <c r="C24" s="22">
         <v>881</v>
       </c>
-      <c r="D24" s="28" t="s">
+      <c r="D24" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="E24" s="27">
-        <v>3</v>
-      </c>
-      <c r="F24" s="27" t="s">
+      <c r="E24" s="22">
+        <v>3</v>
+      </c>
+      <c r="F24" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="G24" s="27" t="s">
+      <c r="G24" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="H24" s="27"/>
-      <c r="I24" s="28"/>
-      <c r="J24" s="27"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1995,12 +2012,12 @@
       <c r="A12" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>

</xml_diff>

<commit_message>
UNED - Principios de Administracion - Trabajo 1
</commit_message>
<xml_diff>
--- a/Plan_Ingenieria_Informatica.xlsx
+++ b/Plan_Ingenieria_Informatica.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jrodrigue253\Github\UNED\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B18CA6-32C1-4E92-884C-A0032CE4242D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B4C758-E4A3-4A75-94F9-6F0B95577D9E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2400" windowWidth="29040" windowHeight="15840" xr2:uid="{8230E5AE-A8B0-403C-B098-7F142039F630}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8230E5AE-A8B0-403C-B098-7F142039F630}"/>
   </bookViews>
   <sheets>
     <sheet name="Diplomado" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="93">
   <si>
     <t>Bloque</t>
   </si>
@@ -311,6 +311,9 @@
   </si>
   <si>
     <t>IIIC2021</t>
+  </si>
+  <si>
+    <t>Total de créditos</t>
   </si>
 </sst>
 </file>
@@ -436,7 +439,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -531,6 +534,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -847,10 +853,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD8781F1-B9E9-4C62-8830-019F772FBC45}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1041,7 +1047,9 @@
       <c r="I7" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="J7" s="24"/>
+      <c r="J7" s="24">
+        <v>10</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="17">
@@ -1438,6 +1446,15 @@
       <c r="H24" s="21"/>
       <c r="I24" s="22"/>
       <c r="J24" s="21"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D25" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="E25" s="5">
+        <f>SUM(E2:E24)</f>
+        <v>78</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1454,10 +1471,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA12924-F294-4484-86F1-E460BC0E3C72}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1833,6 +1850,15 @@
       <c r="G16" s="5"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C17" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="5">
+        <f>SUM(D2:D16)</f>
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>